<commit_message>
fix import and auto approval bug
</commit_message>
<xml_diff>
--- a/ehtest-integration/src/test/data/excel/organization_owner_template.xlsx
+++ b/ehtest-integration/src/test/data/excel/organization_owner_template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <r>
       <rPr>
@@ -276,18 +276,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2016-01-02</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -333,10 +321,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1-101</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>男</t>
   </si>
   <si>
@@ -352,6 +336,26 @@
   </si>
   <si>
     <t>13800138011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,7 +849,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N1"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -937,13 +941,13 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>27</v>
@@ -978,45 +982,45 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="24.95" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
@@ -1025,37 +1029,37 @@
         <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="24.95" customHeight="1">
@@ -1066,43 +1070,43 @@
     </row>
     <row r="7" spans="1:14" ht="24.95" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="24.95" customHeight="1">

</xml_diff>